<commit_message>
update export excel user
</commit_message>
<xml_diff>
--- a/src/public/files/ListUser.xlsx
+++ b/src/public/files/ListUser.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA2E817-EF83-417D-BD63-B8AB7D19B493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3ED31F1-1B8D-441E-BD41-361C2F939410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -600,7 +600,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.35"/>

</xml_diff>